<commit_message>
Small fixes in BOM.xlsx
</commit_message>
<xml_diff>
--- a/hardware/BOM.xlsx
+++ b/hardware/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johannes/Documents/Bastelzeug/Projekte/Wunderkiste/hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CBD0BF88-2A96-0D42-A587-CBD168BE8A55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E4CE52-B2EE-E44C-BA48-855232FDCBD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="460" windowWidth="28240" windowHeight="16560" xr2:uid="{DBBD3A6D-0FFE-2248-96E5-A264D4ADE7FD}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{39D9B7B1-D392-DD4A-AA8F-EDE886E373C5}" name="Wunderkiste" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/johannes/Documents/Bastelzeug/Projekte/Wunderkiste/hardware/pcb_kicad/Wunderkiste.csv" decimal="," thousands="." tab="0" comma="1">
+    <textPr sourceFile="/Users/johannes/Documents/Bastelzeug/Projekte/Wunderkiste/hardware/pcb_kicad/Wunderkiste.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="211">
   <si>
     <t>Hammond 1591XXEBK</t>
   </si>
@@ -473,9 +473,6 @@
     <t>IDC Shrouded pinheader 2x8</t>
   </si>
   <si>
-    <t>IDC Socker 2x8</t>
-  </si>
-  <si>
     <t>WSL 16G</t>
   </si>
   <si>
@@ -524,9 +521,6 @@
     <t>VIS SG 8210</t>
   </si>
   <si>
-    <t>PCB Material for the speaker covers</t>
-  </si>
-  <si>
     <t>EP2CU 160X100</t>
   </si>
   <si>
@@ -647,8 +641,41 @@
     <t>way too long. Maybe you have some leftover IDC cable from another project?</t>
   </si>
   <si>
+    <t>Any metal mesh will do. Cheap alternative: Frying Pan Grease Splash Guard</t>
+  </si>
+  <si>
+    <t>RND 455-00518</t>
+  </si>
+  <si>
+    <t>pack of 55… some felt furniture feet will also work.</t>
+  </si>
+  <si>
+    <t>Rubber feet with adhesive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J3 J9 </t>
+  </si>
+  <si>
+    <t>SW3 SW4 J8 J11</t>
+  </si>
+  <si>
+    <t>SW1 SW 2</t>
+  </si>
+  <si>
+    <t>Molex KK or similar, 2.54mm pin spacing</t>
+  </si>
+  <si>
+    <t>IDC Socket 2x8</t>
+  </si>
+  <si>
+    <t>2.54mm pin spacing</t>
+  </si>
+  <si>
+    <t>2.54mm pin spacing; for the STM32F4 Discovery board</t>
+  </si>
+  <si>
     <r>
-      <t>Attention: Buy version number MB997</t>
+      <t>Attention: Buy brand new so that you get one with version number MB997</t>
     </r>
     <r>
       <rPr>
@@ -669,29 +696,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> for MUCH simpler drag&amp;drop programming</t>
+      <t xml:space="preserve"> for MUCH simpler drag&amp;drop programming.</t>
     </r>
   </si>
   <si>
-    <t>Any metal mesh will do. Cheap alternative: Frying Pan Grease Splash Guard</t>
-  </si>
-  <si>
-    <t>RND 455-00518</t>
-  </si>
-  <si>
-    <t>pack of 55… some felt furniture feet will also work.</t>
-  </si>
-  <si>
-    <t>Rubber feet with adhesive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J3 J9 </t>
-  </si>
-  <si>
-    <t>SW3 SW4 J8 J11</t>
-  </si>
-  <si>
-    <t>SW1 SW 2</t>
+    <t>PCB material for the speaker covers</t>
   </si>
 </sst>
 </file>
@@ -804,13 +813,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1132,8 +1141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4128CDF2-C759-F54C-B3D8-39A7D29F1BEC}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1174,7 +1183,7 @@
         <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1260,7 +1269,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F5" s="5">
         <v>0.123</v>
@@ -1273,7 +1282,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>98</v>
@@ -1368,10 +1377,10 @@
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="10" t="s">
         <v>130</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1393,8 +1402,8 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="4" t="s">
         <v>134</v>
       </c>
@@ -1414,10 +1423,10 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="10" t="s">
         <v>125</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1437,10 +1446,13 @@
         <v>0.09</v>
       </c>
       <c r="H12" s="4"/>
+      <c r="I12" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="4" t="s">
         <v>128</v>
       </c>
@@ -1458,6 +1470,9 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H13" s="4"/>
+      <c r="I13" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
@@ -1533,12 +1548,15 @@
         <v>0.25</v>
       </c>
       <c r="H16" s="4"/>
+      <c r="I16" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="10" t="s">
         <v>131</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -1548,7 +1566,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F17" s="5">
         <v>0.14000000000000001</v>
@@ -1558,18 +1576,21 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="H17" s="4"/>
+      <c r="I17" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="4" t="s">
-        <v>142</v>
+        <v>206</v>
       </c>
       <c r="D18" s="4">
         <v>2</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F18" s="5">
         <v>0.18</v>
@@ -1579,12 +1600,15 @@
         <v>0.36</v>
       </c>
       <c r="H18" s="4"/>
+      <c r="I18" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="B19" s="6" t="s">
+      <c r="A19" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>105</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1604,10 +1628,13 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="H19" s="4"/>
+      <c r="I19" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
       <c r="C20" s="4" t="s">
         <v>106</v>
       </c>
@@ -1625,6 +1652,9 @@
         <v>0.04</v>
       </c>
       <c r="H20" s="4"/>
+      <c r="I20" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
@@ -1663,7 +1693,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F22" s="5">
         <v>8.2000000000000003E-2</v>
@@ -1686,7 +1716,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F23" s="5">
         <v>8.2000000000000003E-2</v>
@@ -1699,7 +1729,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
@@ -1709,7 +1739,7 @@
         <v>6</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F24" s="5">
         <v>8.2000000000000003E-2</v>
@@ -1720,7 +1750,7 @@
       </c>
       <c r="H24" s="4"/>
       <c r="I24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1742,7 +1772,7 @@
       </c>
       <c r="H25" s="4"/>
       <c r="I25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1757,7 +1787,7 @@
         <v>7</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F26" s="5">
         <v>8.2000000000000003E-2</v>
@@ -1776,7 +1806,7 @@
         <v>103</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D27" s="4">
         <v>1</v>
@@ -1791,7 +1821,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>139</v>
@@ -1815,10 +1845,10 @@
       <c r="H28" s="4"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="B29" s="6" t="s">
+      <c r="A29" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>110</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -1840,8 +1870,8 @@
       <c r="H29" s="4"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
       <c r="C30" s="4" t="s">
         <v>112</v>
       </c>
@@ -1865,7 +1895,7 @@
         <v>81</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>82</v>
@@ -1874,7 +1904,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F31" s="5">
         <v>1.7</v>
@@ -1890,7 +1920,7 @@
         <v>83</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>84</v>
@@ -1899,7 +1929,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F32" s="5">
         <v>10.37</v>
@@ -1910,20 +1940,20 @@
       </c>
       <c r="H32" s="4"/>
       <c r="I32" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D33" s="4">
         <v>2</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F33" s="5">
         <v>0.28999999999999998</v>
@@ -1937,16 +1967,16 @@
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D34" s="4">
         <v>1</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F34" s="5">
         <v>2.17</v>
@@ -1960,7 +1990,7 @@
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>86</v>
@@ -1969,7 +1999,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F35" s="5">
         <v>29.75</v>
@@ -1980,7 +2010,7 @@
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="1" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -2004,13 +2034,13 @@
       </c>
       <c r="H36" s="4"/>
       <c r="I36" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>95</v>
@@ -2018,10 +2048,10 @@
       <c r="D37" s="4">
         <v>1</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F37" s="7">
         <v>0.99</v>
       </c>
       <c r="G37" s="5">
@@ -2033,9 +2063,9 @@
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C38" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D38" s="4">
@@ -2078,7 +2108,7 @@
         <v>6</v>
       </c>
       <c r="I39" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -2137,7 +2167,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F42" s="5">
         <v>3.49</v>
@@ -2151,16 +2181,16 @@
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>184</v>
-      </c>
       <c r="D43" s="4">
         <v>1</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F43" s="5">
         <v>2.7</v>
@@ -2171,22 +2201,22 @@
       </c>
       <c r="H43" s="4"/>
       <c r="I43" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D44" s="4">
+        <v>1</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D44" s="4">
-        <v>1</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>185</v>
       </c>
       <c r="F44" s="5">
         <v>1.85</v>
@@ -2197,16 +2227,16 @@
       </c>
       <c r="H44" s="4"/>
       <c r="I44" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -2217,16 +2247,16 @@
       </c>
       <c r="H45" s="4"/>
       <c r="I45" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -2240,16 +2270,16 @@
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
       <c r="B47" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="D47" s="4">
+        <v>1</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="D47" s="4">
-        <v>1</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>158</v>
       </c>
       <c r="F47" s="5">
         <v>8.9499999999999993</v>
@@ -2260,20 +2290,20 @@
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="4">
         <v>1</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F48" s="5">
         <v>0.78</v>
@@ -2287,14 +2317,14 @@
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
       <c r="B49" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="4">
         <v>1</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F49" s="5">
         <v>0.78</v>
@@ -2308,14 +2338,14 @@
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
       <c r="B50" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4">
         <v>1</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F50" s="5">
         <v>0.76</v>
@@ -2329,14 +2359,14 @@
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4">
         <v>1</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F51" s="5">
         <v>5.25</v>
@@ -2347,20 +2377,20 @@
       </c>
       <c r="H51" s="4"/>
       <c r="I51" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
       <c r="B52" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4">
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F52" s="5">
         <v>0.82</v>
@@ -2371,20 +2401,20 @@
       </c>
       <c r="H52" s="4"/>
       <c r="I52" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
       <c r="B53" s="4" t="s">
-        <v>159</v>
+        <v>210</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4">
         <v>1</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F53" s="5">
         <v>2.0499999999999998</v>
@@ -2396,26 +2426,26 @@
       <c r="H53" s="4"/>
     </row>
     <row r="54" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="F54" s="9" t="s">
+      <c r="F54" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="G54" s="10">
+      <c r="G54" s="9">
         <f>SUM(G2:G41)</f>
         <v>110.45499999999998</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="A29:A30"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="A29:A30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>